<commit_message>
User yandex api in registration form
</commit_message>
<xml_diff>
--- a/Мастера.xlsx
+++ b/Мастера.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8205" activeTab="1"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Кировский" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Имя</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>318-45-42</t>
+  </si>
+  <si>
+    <t>Алексей</t>
+  </si>
+  <si>
+    <t>8-905-223-02-49</t>
+  </si>
+  <si>
+    <t>Борис</t>
+  </si>
+  <si>
+    <t>8-962-685-01-80</t>
   </si>
 </sst>
 </file>
@@ -464,16 +476,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,6 +544,22 @@
         <v>20</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>